<commit_message>
get a plot for the historical rpk, minor fix in for the brayton cycle
</commit_message>
<xml_diff>
--- a/database/rawdata/USDOT/Traffic and Operations 1929-Present_Vollständige D_data.xlsx
+++ b/database/rawdata/USDOT/Traffic and Operations 1929-Present_Vollständige D_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRohr\Desktop\Masterarbeit\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRohr\Desktop\Masterarbeit\Python\Aircraft-Performance\database\rawdata\USDOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C9E535B-4B92-4EAC-B1BB-223F3A897B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333AEF27-0936-40C3-A485-5ABF7FDCCE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic and Operations 1929-Pre" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="259">
   <si>
     <t>Year</t>
   </si>
@@ -421,9 +421,6 @@
     <t>0,710701581</t>
   </si>
   <si>
-    <t>3201366,12411332</t>
-  </si>
-  <si>
     <t>24233,637621127</t>
   </si>
   <si>
@@ -451,9 +448,6 @@
     <t>0,692407769</t>
   </si>
   <si>
-    <t>3108526,50651403</t>
-  </si>
-  <si>
     <t>23095,220225902</t>
   </si>
   <si>
@@ -481,9 +475,6 @@
     <t>0,713362113</t>
   </si>
   <si>
-    <t>3124069,1390466</t>
-  </si>
-  <si>
     <t>23816,593624857</t>
   </si>
   <si>
@@ -511,9 +502,6 @@
     <t>0,715767847</t>
   </si>
   <si>
-    <t>3180302,38354944</t>
-  </si>
-  <si>
     <t>26780,987436185</t>
   </si>
   <si>
@@ -541,9 +529,6 @@
     <t>0,733911550</t>
   </si>
   <si>
-    <t>3628725,01962991</t>
-  </si>
-  <si>
     <t>28077,205262432</t>
   </si>
   <si>
@@ -571,9 +556,6 @@
     <t>0,749427571</t>
   </si>
   <si>
-    <t>3919023,0212003</t>
-  </si>
-  <si>
     <t>28776,035742669</t>
   </si>
   <si>
@@ -601,9 +583,6 @@
     <t>0,758150692</t>
   </si>
   <si>
-    <t>4170556,1959147</t>
-  </si>
-  <si>
     <t>29869,367300459</t>
   </si>
   <si>
@@ -631,9 +610,6 @@
     <t>0,768047272</t>
   </si>
   <si>
-    <t>4513095,88653466</t>
-  </si>
-  <si>
     <t>29988,856031948</t>
   </si>
   <si>
@@ -661,9 +637,6 @@
     <t>0,760138426</t>
   </si>
   <si>
-    <t>4608466,25816926</t>
-  </si>
-  <si>
     <t>29372,403867587</t>
   </si>
   <si>
@@ -691,9 +664,6 @@
     <t>0,766817019</t>
   </si>
   <si>
-    <t>4561413,04271906</t>
-  </si>
-  <si>
     <t>30754,207128909</t>
   </si>
   <si>
@@ -719,9 +689,6 @@
   </si>
   <si>
     <t>0,781701864</t>
-  </si>
-  <si>
-    <t>4930250,01571544</t>
   </si>
   <si>
     <t>31767,566386975</t>
@@ -835,7 +802,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1669,11 +1636,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3698,8 +3665,8 @@
       <c r="J73" t="s">
         <v>132</v>
       </c>
-      <c r="K73" t="s">
-        <v>133</v>
+      <c r="K73">
+        <v>3201366</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.75">
@@ -3707,34 +3674,34 @@
         <v>2001</v>
       </c>
       <c r="B74" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" t="s">
         <v>134</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>135</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>136</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>137</v>
       </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>138</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>139</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>140</v>
       </c>
-      <c r="I74" t="s">
+      <c r="J74" t="s">
         <v>141</v>
       </c>
-      <c r="J74" t="s">
-        <v>142</v>
-      </c>
-      <c r="K74" t="s">
-        <v>143</v>
+      <c r="K74">
+        <v>3108526</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.75">
@@ -3742,34 +3709,34 @@
         <v>2002</v>
       </c>
       <c r="B75" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" t="s">
+        <v>143</v>
+      </c>
+      <c r="D75" t="s">
         <v>144</v>
       </c>
-      <c r="C75" t="s">
+      <c r="E75" t="s">
         <v>145</v>
       </c>
-      <c r="D75" t="s">
+      <c r="F75" t="s">
         <v>146</v>
       </c>
-      <c r="E75" t="s">
+      <c r="G75" t="s">
         <v>147</v>
       </c>
-      <c r="F75" t="s">
+      <c r="H75" t="s">
         <v>148</v>
       </c>
-      <c r="G75" t="s">
+      <c r="I75" t="s">
         <v>149</v>
       </c>
-      <c r="H75" t="s">
+      <c r="J75" t="s">
         <v>150</v>
       </c>
-      <c r="I75" t="s">
-        <v>151</v>
-      </c>
-      <c r="J75" t="s">
-        <v>152</v>
-      </c>
-      <c r="K75" t="s">
-        <v>153</v>
+      <c r="K75">
+        <v>3124069</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.75">
@@ -3777,34 +3744,34 @@
         <v>2003</v>
       </c>
       <c r="B76" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" t="s">
+        <v>152</v>
+      </c>
+      <c r="D76" t="s">
+        <v>153</v>
+      </c>
+      <c r="E76" t="s">
         <v>154</v>
       </c>
-      <c r="C76" t="s">
+      <c r="F76" t="s">
         <v>155</v>
       </c>
-      <c r="D76" t="s">
+      <c r="G76" t="s">
         <v>156</v>
       </c>
-      <c r="E76" t="s">
+      <c r="H76" t="s">
         <v>157</v>
       </c>
-      <c r="F76" t="s">
+      <c r="I76" t="s">
         <v>158</v>
       </c>
-      <c r="G76" t="s">
+      <c r="J76" t="s">
         <v>159</v>
       </c>
-      <c r="H76" t="s">
-        <v>160</v>
-      </c>
-      <c r="I76" t="s">
-        <v>161</v>
-      </c>
-      <c r="J76" t="s">
-        <v>162</v>
-      </c>
-      <c r="K76" t="s">
-        <v>163</v>
+      <c r="K76">
+        <v>3180302</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.75">
@@ -3812,34 +3779,34 @@
         <v>2004</v>
       </c>
       <c r="B77" t="s">
+        <v>160</v>
+      </c>
+      <c r="C77" t="s">
+        <v>161</v>
+      </c>
+      <c r="D77" t="s">
+        <v>162</v>
+      </c>
+      <c r="E77" t="s">
+        <v>163</v>
+      </c>
+      <c r="F77" t="s">
         <v>164</v>
       </c>
-      <c r="C77" t="s">
+      <c r="G77" t="s">
         <v>165</v>
       </c>
-      <c r="D77" t="s">
+      <c r="H77" t="s">
         <v>166</v>
       </c>
-      <c r="E77" t="s">
+      <c r="I77" t="s">
         <v>167</v>
       </c>
-      <c r="F77" t="s">
+      <c r="J77" t="s">
         <v>168</v>
       </c>
-      <c r="G77" t="s">
-        <v>169</v>
-      </c>
-      <c r="H77" t="s">
-        <v>170</v>
-      </c>
-      <c r="I77" t="s">
-        <v>171</v>
-      </c>
-      <c r="J77" t="s">
-        <v>172</v>
-      </c>
-      <c r="K77" t="s">
-        <v>173</v>
+      <c r="K77">
+        <v>3628725</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.75">
@@ -3847,34 +3814,34 @@
         <v>2005</v>
       </c>
       <c r="B78" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" t="s">
+        <v>170</v>
+      </c>
+      <c r="D78" t="s">
+        <v>171</v>
+      </c>
+      <c r="E78" t="s">
+        <v>172</v>
+      </c>
+      <c r="F78" t="s">
+        <v>173</v>
+      </c>
+      <c r="G78" t="s">
         <v>174</v>
       </c>
-      <c r="C78" t="s">
+      <c r="H78" t="s">
         <v>175</v>
       </c>
-      <c r="D78" t="s">
+      <c r="I78" t="s">
         <v>176</v>
       </c>
-      <c r="E78" t="s">
+      <c r="J78" t="s">
         <v>177</v>
       </c>
-      <c r="F78" t="s">
-        <v>178</v>
-      </c>
-      <c r="G78" t="s">
-        <v>179</v>
-      </c>
-      <c r="H78" t="s">
-        <v>180</v>
-      </c>
-      <c r="I78" t="s">
-        <v>181</v>
-      </c>
-      <c r="J78" t="s">
-        <v>182</v>
-      </c>
-      <c r="K78" t="s">
-        <v>183</v>
+      <c r="K78">
+        <v>3919023</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.75">
@@ -3882,34 +3849,34 @@
         <v>2006</v>
       </c>
       <c r="B79" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" t="s">
+        <v>179</v>
+      </c>
+      <c r="D79" t="s">
+        <v>180</v>
+      </c>
+      <c r="E79" t="s">
+        <v>181</v>
+      </c>
+      <c r="F79" t="s">
+        <v>182</v>
+      </c>
+      <c r="G79" t="s">
+        <v>183</v>
+      </c>
+      <c r="H79" t="s">
         <v>184</v>
       </c>
-      <c r="C79" t="s">
+      <c r="I79" t="s">
         <v>185</v>
       </c>
-      <c r="D79" t="s">
+      <c r="J79" t="s">
         <v>186</v>
       </c>
-      <c r="E79" t="s">
-        <v>187</v>
-      </c>
-      <c r="F79" t="s">
-        <v>188</v>
-      </c>
-      <c r="G79" t="s">
-        <v>189</v>
-      </c>
-      <c r="H79" t="s">
-        <v>190</v>
-      </c>
-      <c r="I79" t="s">
-        <v>191</v>
-      </c>
-      <c r="J79" t="s">
-        <v>192</v>
-      </c>
-      <c r="K79" t="s">
-        <v>193</v>
+      <c r="K79">
+        <v>4170556</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.75">
@@ -3917,34 +3884,34 @@
         <v>2007</v>
       </c>
       <c r="B80" t="s">
+        <v>187</v>
+      </c>
+      <c r="C80" t="s">
+        <v>188</v>
+      </c>
+      <c r="D80" t="s">
+        <v>189</v>
+      </c>
+      <c r="E80" t="s">
+        <v>190</v>
+      </c>
+      <c r="F80" t="s">
+        <v>191</v>
+      </c>
+      <c r="G80" t="s">
+        <v>192</v>
+      </c>
+      <c r="H80" t="s">
+        <v>193</v>
+      </c>
+      <c r="I80" t="s">
         <v>194</v>
       </c>
-      <c r="C80" t="s">
+      <c r="J80" t="s">
         <v>195</v>
       </c>
-      <c r="D80" t="s">
-        <v>196</v>
-      </c>
-      <c r="E80" t="s">
-        <v>197</v>
-      </c>
-      <c r="F80" t="s">
-        <v>198</v>
-      </c>
-      <c r="G80" t="s">
-        <v>199</v>
-      </c>
-      <c r="H80" t="s">
-        <v>200</v>
-      </c>
-      <c r="I80" t="s">
-        <v>201</v>
-      </c>
-      <c r="J80" t="s">
-        <v>202</v>
-      </c>
-      <c r="K80" t="s">
-        <v>203</v>
+      <c r="K80">
+        <v>4513095</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.75">
@@ -3952,34 +3919,34 @@
         <v>2008</v>
       </c>
       <c r="B81" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" t="s">
+        <v>197</v>
+      </c>
+      <c r="D81" t="s">
+        <v>198</v>
+      </c>
+      <c r="E81" t="s">
+        <v>199</v>
+      </c>
+      <c r="F81" t="s">
+        <v>200</v>
+      </c>
+      <c r="G81" t="s">
+        <v>201</v>
+      </c>
+      <c r="H81" t="s">
+        <v>202</v>
+      </c>
+      <c r="I81" t="s">
+        <v>203</v>
+      </c>
+      <c r="J81" t="s">
         <v>204</v>
       </c>
-      <c r="C81" t="s">
-        <v>205</v>
-      </c>
-      <c r="D81" t="s">
-        <v>206</v>
-      </c>
-      <c r="E81" t="s">
-        <v>207</v>
-      </c>
-      <c r="F81" t="s">
-        <v>208</v>
-      </c>
-      <c r="G81" t="s">
-        <v>209</v>
-      </c>
-      <c r="H81" t="s">
-        <v>210</v>
-      </c>
-      <c r="I81" t="s">
-        <v>211</v>
-      </c>
-      <c r="J81" t="s">
-        <v>212</v>
-      </c>
-      <c r="K81" t="s">
-        <v>213</v>
+      <c r="K81">
+        <v>4608466</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.75">
@@ -3987,34 +3954,34 @@
         <v>2009</v>
       </c>
       <c r="B82" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C82" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D82" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E82" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F82" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="G82" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H82" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="I82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J82" t="s">
-        <v>222</v>
-      </c>
-      <c r="K82" t="s">
-        <v>223</v>
+        <v>213</v>
+      </c>
+      <c r="K82">
+        <v>4561413</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.75">
@@ -4022,34 +3989,34 @@
         <v>2010</v>
       </c>
       <c r="B83" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C83" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D83" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E83" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F83" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="G83" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="H83" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="I83" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="J83" t="s">
-        <v>232</v>
-      </c>
-      <c r="K83" t="s">
-        <v>233</v>
+        <v>222</v>
+      </c>
+      <c r="K83">
+        <v>4930250</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.75">
@@ -4057,10 +4024,10 @@
         <v>2011</v>
       </c>
       <c r="B84" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="C84" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D84">
         <v>6747537</v>
@@ -4072,7 +4039,7 @@
         <v>190690</v>
       </c>
       <c r="G84" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="H84">
         <v>4913</v>
@@ -4081,7 +4048,7 @@
         <v>2883</v>
       </c>
       <c r="J84" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="K84">
         <v>5263525</v>
@@ -4092,10 +4059,10 @@
         <v>2012</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C85" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D85">
         <v>7021134</v>
@@ -4107,7 +4074,7 @@
         <v>188712</v>
       </c>
       <c r="G85" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="H85">
         <v>5149</v>
@@ -4116,7 +4083,7 @@
         <v>3013</v>
       </c>
       <c r="J85" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="K85">
         <v>5537024</v>
@@ -4127,10 +4094,10 @@
         <v>2013</v>
       </c>
       <c r="B86" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C86" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="D86">
         <v>7349025</v>
@@ -4142,7 +4109,7 @@
         <v>189463</v>
       </c>
       <c r="G86" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="H86">
         <v>5537</v>
@@ -4151,7 +4118,7 @@
         <v>3148</v>
       </c>
       <c r="J86" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="K86">
         <v>5841156</v>
@@ -4162,10 +4129,10 @@
         <v>2014</v>
       </c>
       <c r="B87" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="C87" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="D87">
         <v>7765176</v>
@@ -4177,7 +4144,7 @@
         <v>198283</v>
       </c>
       <c r="G87" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="H87">
         <v>6022</v>
@@ -4186,7 +4153,7 @@
         <v>3327</v>
       </c>
       <c r="J87" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="K87">
         <v>6190282</v>
@@ -4197,10 +4164,10 @@
         <v>2015</v>
       </c>
       <c r="B88" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C88" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="D88">
         <v>8293327</v>
@@ -4212,7 +4179,7 @@
         <v>200828</v>
       </c>
       <c r="G88" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="H88">
         <v>6491</v>
@@ -4221,7 +4188,7 @@
         <v>3567</v>
       </c>
       <c r="J88" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="K88">
         <v>6654454</v>
@@ -4232,10 +4199,10 @@
         <v>2016</v>
       </c>
       <c r="B89" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C89" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D89">
         <v>8901086</v>
@@ -4247,7 +4214,7 @@
         <v>208016</v>
       </c>
       <c r="G89" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="H89">
         <v>6622</v>
@@ -4256,7 +4223,7 @@
         <v>3806</v>
       </c>
       <c r="J89" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="K89">
         <v>7146283</v>
@@ -4267,10 +4234,10 @@
         <v>2017</v>
       </c>
       <c r="B90" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C90" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D90">
         <v>9473126</v>
@@ -4282,7 +4249,7 @@
         <v>227177</v>
       </c>
       <c r="G90" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="H90">
         <v>7383</v>
@@ -4291,7 +4258,7 @@
         <v>4075</v>
       </c>
       <c r="J90" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="K90">
         <v>7718470</v>
@@ -4302,10 +4269,10 @@
         <v>2018</v>
       </c>
       <c r="B91" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C91" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="D91">
         <v>10147668</v>
@@ -4326,7 +4293,7 @@
         <v>4341</v>
       </c>
       <c r="J91" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="K91">
         <v>8280851</v>
@@ -4361,7 +4328,7 @@
         <v>4490</v>
       </c>
       <c r="J92" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="K92">
         <v>8664032</v>
@@ -4387,7 +4354,7 @@
         <v>192824</v>
       </c>
       <c r="G93" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="H93">
         <v>4900</v>
@@ -4396,7 +4363,7 @@
         <v>1782</v>
       </c>
       <c r="J93" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="K93">
         <v>2962287</v>
@@ -4422,7 +4389,7 @@
         <v>231635</v>
       </c>
       <c r="G94" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="H94">
         <v>4265</v>
@@ -4431,7 +4398,7 @@
         <v>2284</v>
       </c>
       <c r="J94" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="K94">
         <v>3626024</v>

</xml_diff>